<commit_message>
moved database variables to global
</commit_message>
<xml_diff>
--- a/Middleware Design/Userform-to-table-description.xlsx
+++ b/Middleware Design/Userform-to-table-description.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Evelyn\Education\CSC 499 - Pharm Internship\CSC 499 - Pharm Internship\FINAL solution\Middleware Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2142456A-35E0-40CE-975A-A6120EFC9866}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9937FA25-A931-4DDC-9AC4-DAFA176D101A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{52C3DF51-53F1-45DC-9701-BFA6EF7713A5}"/>
+    <workbookView xWindow="570" yWindow="330" windowWidth="18600" windowHeight="9230" xr2:uid="{52C3DF51-53F1-45DC-9701-BFA6EF7713A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="196">
   <si>
     <t>UserForm Object</t>
   </si>
@@ -57,9 +57,6 @@
     <t>No -- only one field in the tuple</t>
   </si>
   <si>
-    <t xml:space="preserve">Begin Session Form &gt; Date &amp; Times </t>
-  </si>
-  <si>
     <t>Session &gt; Date &amp; Times Fields</t>
   </si>
   <si>
@@ -1436,14 +1433,143 @@
     <t xml:space="preserve">Diabetes education </t>
   </si>
   <si>
-    <t xml:space="preserve">Welcome Screen &gt; Session Type </t>
+    <t>Global Variables</t>
+  </si>
+  <si>
+    <t>Welcome Screen &gt; Session Type All Session Types</t>
+  </si>
+  <si>
+    <t>Begin Session Form &gt; Date &amp; Times                                                  All Session Types</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Georgia"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Yes </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Georgia"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">- session type, date, rph, prep, start, end, session time, document, reason </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Georgia"/>
+        <family val="1"/>
+      </rPr>
+      <t>Yes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Georgia"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - session type</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Georgia"/>
+        <family val="1"/>
+      </rPr>
+      <t>No</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Georgia"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Georgia"/>
+        <family val="1"/>
+      </rPr>
+      <t>Yes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Georgia"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, but both must be updated at the same time </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">No </t>
+  </si>
+  <si>
+    <t>Userform Object Variables</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Yes - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Georgia"/>
+        <family val="1"/>
+      </rPr>
+      <t>temporary storage until updated to global variables - no user information yet to create a patient</t>
+    </r>
+  </si>
+  <si>
+    <t>Yes - temporary storage until updated to global variables - no user information yet to create a patient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes - session type, date, rph, prep, start, end, session time, document, reason </t>
+  </si>
+  <si>
+    <r>
+      <t>Yes -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Georgia"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> temporary storage until updated to global variables - no user information yet to create a patient</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1467,6 +1593,27 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1476,7 +1623,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1541,11 +1688,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1580,15 +1736,67 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1904,22 +2112,25 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DEB8B88-B536-4BC6-99B2-FA508FDDE9AC}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D153"/>
+  <dimension ref="A1:G153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E35" sqref="E35:E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.81640625" customWidth="1"/>
     <col min="2" max="2" width="40.90625" customWidth="1"/>
     <col min="3" max="3" width="18.36328125" customWidth="1"/>
     <col min="4" max="4" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.81640625" style="33" customWidth="1"/>
+    <col min="6" max="6" width="17.36328125" style="34" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1932,1357 +2143,1946 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="E1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="G1" s="22"/>
+    </row>
+    <row r="2" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="13" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-    </row>
-    <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="E2" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="G2" s="20"/>
+    </row>
+    <row r="3" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="15"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="20"/>
+    </row>
+    <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="G4" s="17"/>
+    </row>
+    <row r="5" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="15"/>
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="14" t="s">
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="17"/>
+    </row>
+    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-    </row>
-    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="G6" s="24"/>
+    </row>
+    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="24"/>
+    </row>
+    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-    </row>
-    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="24"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="24"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="6"/>
       <c r="B10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="24"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="6"/>
       <c r="B11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="24"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="6"/>
       <c r="B12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-    </row>
-    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>20</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="24"/>
+    </row>
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="7"/>
       <c r="B13" s="5"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-    </row>
-    <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="24"/>
+    </row>
+    <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="G14" s="24"/>
+    </row>
+    <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="24"/>
+    </row>
+    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-    </row>
-    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="B16" s="8"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-    </row>
-    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="24"/>
+    </row>
+    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="9"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-    </row>
-    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="24"/>
+    </row>
+    <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="F18" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="G18" s="24"/>
+    </row>
+    <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="24"/>
+    </row>
+    <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-    </row>
-    <row r="20" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="B20" s="8"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-    </row>
-    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="24"/>
+    </row>
+    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B21" s="9"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-    </row>
-    <row r="22" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="24"/>
+    </row>
+    <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="G22" s="24"/>
+    </row>
+    <row r="23" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B23" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="24"/>
+    </row>
+    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-    </row>
-    <row r="24" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="24"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-    </row>
-    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>42</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="24"/>
+    </row>
+    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="7"/>
       <c r="B26" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-    </row>
-    <row r="27" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="24"/>
+    </row>
+    <row r="27" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="G27" s="24"/>
+    </row>
+    <row r="28" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="24"/>
+    </row>
+    <row r="29" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-    </row>
-    <row r="29" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="24"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-    </row>
-    <row r="31" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="24"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="6"/>
       <c r="B31" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-    </row>
-    <row r="32" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="24"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="6"/>
       <c r="B32" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="24"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="6"/>
       <c r="B33" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-    </row>
-    <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>54</v>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="24"/>
+    </row>
+    <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="7"/>
       <c r="B34" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="24"/>
+    </row>
+    <row r="35" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-    </row>
-    <row r="35" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
+      <c r="B35" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="30"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="24"/>
+    </row>
+    <row r="36" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B36" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C35" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="24"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
       <c r="B37" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="24"/>
+    </row>
+    <row r="38" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-    </row>
-    <row r="38" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="24"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="6"/>
       <c r="B39" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="24"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="6"/>
       <c r="B40" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="24"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="6"/>
       <c r="B41" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="24"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="6"/>
       <c r="B42" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="24"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="6"/>
       <c r="B43" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="24"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="6"/>
       <c r="B44" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="32"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="24"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="6"/>
       <c r="B45" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="25"/>
+      <c r="G45" s="24"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="6"/>
       <c r="B46" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="25"/>
+      <c r="G46" s="24"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="6"/>
       <c r="B47" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="24"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="6"/>
       <c r="B48" s="4"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-    </row>
-    <row r="49" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="32"/>
+      <c r="F48" s="25"/>
+      <c r="G48" s="24"/>
+    </row>
+    <row r="49" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="7"/>
       <c r="B49" s="5"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" s="14" t="s">
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="25"/>
+      <c r="G49" s="24"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B50" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="C50" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E50" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="F50" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="G50" s="24"/>
+    </row>
+    <row r="51" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A51" s="13"/>
+      <c r="B51" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E51" s="32"/>
+      <c r="F51" s="25"/>
+      <c r="G51" s="24"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A52" s="13"/>
+      <c r="B52" s="10" t="s">
         <v>75</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A51" s="12"/>
-      <c r="B51" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" s="12"/>
-      <c r="B52" s="10" t="s">
-        <v>76</v>
       </c>
       <c r="C52" s="8"/>
       <c r="D52" s="4"/>
-    </row>
-    <row r="53" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A53" s="12"/>
+      <c r="E52" s="32"/>
+      <c r="F52" s="25"/>
+      <c r="G52" s="24"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53" s="13"/>
       <c r="B53" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
-    </row>
-    <row r="54" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A54" s="12"/>
+      <c r="E53" s="32"/>
+      <c r="F53" s="25"/>
+      <c r="G53" s="24"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54" s="13"/>
       <c r="B54" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" s="12"/>
+      <c r="E54" s="32"/>
+      <c r="F54" s="25"/>
+      <c r="G54" s="24"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A55" s="13"/>
       <c r="B55" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56" s="12"/>
+      <c r="E55" s="32"/>
+      <c r="F55" s="25"/>
+      <c r="G55" s="24"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56" s="13"/>
       <c r="B56" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57" s="12"/>
+      <c r="E56" s="32"/>
+      <c r="F56" s="25"/>
+      <c r="G56" s="24"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A57" s="13"/>
       <c r="B57" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A58" s="12"/>
+      <c r="E57" s="32"/>
+      <c r="F57" s="25"/>
+      <c r="G57" s="24"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58" s="13"/>
       <c r="B58" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
-    </row>
-    <row r="59" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A59" s="12"/>
+      <c r="E58" s="32"/>
+      <c r="F58" s="25"/>
+      <c r="G58" s="24"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59" s="13"/>
       <c r="B59" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A60" s="12"/>
+      <c r="E59" s="32"/>
+      <c r="F59" s="25"/>
+      <c r="G59" s="24"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A60" s="13"/>
       <c r="B60" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A61" s="12"/>
+      <c r="E60" s="32"/>
+      <c r="F60" s="25"/>
+      <c r="G60" s="24"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A61" s="13"/>
       <c r="B61" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A62" s="12"/>
+      <c r="E61" s="32"/>
+      <c r="F61" s="25"/>
+      <c r="G61" s="24"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A62" s="13"/>
       <c r="B62" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C62" s="8"/>
       <c r="D62" s="8"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A63" s="12"/>
+      <c r="E62" s="32"/>
+      <c r="F62" s="25"/>
+      <c r="G62" s="24"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63" s="13"/>
       <c r="B63" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A64" s="12"/>
+      <c r="E63" s="32"/>
+      <c r="F63" s="25"/>
+      <c r="G63" s="24"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A64" s="13"/>
       <c r="B64" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
-    </row>
-    <row r="65" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A65" s="12"/>
+      <c r="E64" s="32"/>
+      <c r="F64" s="25"/>
+      <c r="G64" s="24"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A65" s="13"/>
       <c r="B65" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
-    </row>
-    <row r="66" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A66" s="12"/>
+      <c r="E65" s="32"/>
+      <c r="F65" s="25"/>
+      <c r="G65" s="24"/>
+    </row>
+    <row r="66" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A66" s="13"/>
       <c r="B66" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
-    </row>
-    <row r="67" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A67" s="12"/>
+      <c r="E66" s="32"/>
+      <c r="F66" s="25"/>
+      <c r="G66" s="24"/>
+    </row>
+    <row r="67" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A67" s="13"/>
       <c r="B67" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
-    </row>
-    <row r="68" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A68" s="12"/>
+      <c r="E67" s="32"/>
+      <c r="F67" s="25"/>
+      <c r="G67" s="24"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A68" s="13"/>
       <c r="B68" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C68" s="8"/>
       <c r="D68" s="8"/>
-    </row>
-    <row r="69" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A69" s="12"/>
+      <c r="E68" s="32"/>
+      <c r="F68" s="25"/>
+      <c r="G68" s="24"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A69" s="13"/>
       <c r="B69" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C69" s="8"/>
       <c r="D69" s="8"/>
-    </row>
-    <row r="70" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="13"/>
+      <c r="E69" s="32"/>
+      <c r="F69" s="25"/>
+      <c r="G69" s="24"/>
+    </row>
+    <row r="70" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A70" s="14"/>
       <c r="B70" s="5"/>
       <c r="C70" s="9"/>
       <c r="D70" s="9"/>
-    </row>
-    <row r="71" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E70" s="31"/>
+      <c r="F70" s="25"/>
+      <c r="G70" s="24"/>
+    </row>
+    <row r="71" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C71" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D71" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E71" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="F71" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="G71" s="24"/>
+    </row>
+    <row r="72" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A72" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B72" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C71" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="D71" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A72" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C72" s="12"/>
-      <c r="D72" s="12"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C72" s="13"/>
+      <c r="D72" s="13"/>
+      <c r="E72" s="32"/>
+      <c r="F72" s="25"/>
+      <c r="G72" s="24"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" s="2"/>
       <c r="B73" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C73" s="12"/>
-      <c r="D73" s="12"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+      <c r="C73" s="13"/>
+      <c r="D73" s="13"/>
+      <c r="E73" s="32"/>
+      <c r="F73" s="25"/>
+      <c r="G73" s="24"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" s="6"/>
       <c r="B74" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C74" s="12"/>
-      <c r="D74" s="12"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+      <c r="C74" s="13"/>
+      <c r="D74" s="13"/>
+      <c r="E74" s="32"/>
+      <c r="F74" s="25"/>
+      <c r="G74" s="24"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" s="6"/>
       <c r="B75" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C75" s="12"/>
-      <c r="D75" s="12"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+      <c r="C75" s="13"/>
+      <c r="D75" s="13"/>
+      <c r="E75" s="32"/>
+      <c r="F75" s="25"/>
+      <c r="G75" s="24"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" s="6"/>
       <c r="B76" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
-    </row>
-    <row r="77" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>103</v>
+      </c>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
+      <c r="E76" s="32"/>
+      <c r="F76" s="25"/>
+      <c r="G76" s="24"/>
+    </row>
+    <row r="77" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A77" s="7"/>
       <c r="B77" s="5"/>
-      <c r="C77" s="13"/>
-      <c r="D77" s="13"/>
-    </row>
-    <row r="78" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="C77" s="14"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="31"/>
+      <c r="F77" s="25"/>
+      <c r="G77" s="24"/>
+    </row>
+    <row r="78" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C78" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="D78" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E78" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="F78" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="G78" s="24"/>
+    </row>
+    <row r="79" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A79" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B79" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C78" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="D78" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A79" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C79" s="12"/>
-      <c r="D79" s="12"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C79" s="13"/>
+      <c r="D79" s="13"/>
+      <c r="E79" s="32"/>
+      <c r="F79" s="25"/>
+      <c r="G79" s="24"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" s="6"/>
       <c r="B80" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C80" s="12"/>
-      <c r="D80" s="12"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+      <c r="C80" s="13"/>
+      <c r="D80" s="13"/>
+      <c r="E80" s="32"/>
+      <c r="F80" s="25"/>
+      <c r="G80" s="24"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" s="6"/>
       <c r="B81" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C81" s="12"/>
-      <c r="D81" s="12"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+      <c r="C81" s="13"/>
+      <c r="D81" s="13"/>
+      <c r="E81" s="32"/>
+      <c r="F81" s="25"/>
+      <c r="G81" s="24"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" s="6"/>
       <c r="B82" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C82" s="12"/>
-      <c r="D82" s="12"/>
-    </row>
-    <row r="83" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>111</v>
+      </c>
+      <c r="C82" s="13"/>
+      <c r="D82" s="13"/>
+      <c r="E82" s="32"/>
+      <c r="F82" s="25"/>
+      <c r="G82" s="24"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" s="6"/>
       <c r="B83" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C83" s="12"/>
-      <c r="D83" s="12"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+      <c r="C83" s="13"/>
+      <c r="D83" s="13"/>
+      <c r="E83" s="32"/>
+      <c r="F83" s="25"/>
+      <c r="G83" s="24"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" s="6"/>
       <c r="B84" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C84" s="12"/>
-      <c r="D84" s="12"/>
-    </row>
-    <row r="85" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>113</v>
+      </c>
+      <c r="C84" s="13"/>
+      <c r="D84" s="13"/>
+      <c r="E84" s="32"/>
+      <c r="F84" s="25"/>
+      <c r="G84" s="24"/>
+    </row>
+    <row r="85" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A85" s="7"/>
       <c r="B85" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C85" s="13"/>
-      <c r="D85" s="13"/>
-    </row>
-    <row r="86" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A86" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C85" s="14"/>
+      <c r="D85" s="14"/>
+      <c r="E85" s="31"/>
+      <c r="F85" s="25"/>
+      <c r="G85" s="24"/>
+    </row>
+    <row r="86" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A86" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B86" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="C86" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D86" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="E86" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="F86" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="G86" s="24"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A87" s="13"/>
+      <c r="B87" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="C86" s="4" t="s">
+      <c r="C87" s="4"/>
+      <c r="D87" s="13"/>
+      <c r="E87" s="32"/>
+      <c r="F87" s="25"/>
+      <c r="G87" s="24"/>
+    </row>
+    <row r="88" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A88" s="13"/>
+      <c r="B88" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C88" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D86" s="14" t="s">
+      <c r="D88" s="13"/>
+      <c r="E88" s="32"/>
+      <c r="F88" s="25"/>
+      <c r="G88" s="24"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A89" s="13"/>
+      <c r="B89" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C89" s="8"/>
+      <c r="D89" s="13"/>
+      <c r="E89" s="32"/>
+      <c r="F89" s="25"/>
+      <c r="G89" s="24"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A90" s="13"/>
+      <c r="B90" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C90" s="8"/>
+      <c r="D90" s="13"/>
+      <c r="E90" s="32"/>
+      <c r="F90" s="25"/>
+      <c r="G90" s="24"/>
+    </row>
+    <row r="91" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A91" s="14"/>
+      <c r="B91" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C91" s="9"/>
+      <c r="D91" s="14"/>
+      <c r="E91" s="31"/>
+      <c r="F91" s="25"/>
+      <c r="G91" s="24"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A92" s="12" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A87" s="12"/>
-      <c r="B87" s="10" t="s">
+      <c r="B92" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C92" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D92" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E92" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="F92" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="G92" s="24"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A93" s="13"/>
+      <c r="B93" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C93" s="13"/>
+      <c r="D93" s="13"/>
+      <c r="E93" s="32"/>
+      <c r="F93" s="25"/>
+      <c r="G93" s="24"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A94" s="13"/>
+      <c r="B94" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C94" s="13"/>
+      <c r="D94" s="13"/>
+      <c r="E94" s="32"/>
+      <c r="F94" s="25"/>
+      <c r="G94" s="24"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A95" s="13"/>
+      <c r="B95" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C95" s="13"/>
+      <c r="D95" s="13"/>
+      <c r="E95" s="32"/>
+      <c r="F95" s="25"/>
+      <c r="G95" s="24"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A96" s="13"/>
+      <c r="B96" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C96" s="13"/>
+      <c r="D96" s="13"/>
+      <c r="E96" s="32"/>
+      <c r="F96" s="25"/>
+      <c r="G96" s="24"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A97" s="13"/>
+      <c r="B97" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C97" s="13"/>
+      <c r="D97" s="13"/>
+      <c r="E97" s="32"/>
+      <c r="F97" s="25"/>
+      <c r="G97" s="24"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A98" s="13"/>
+      <c r="B98" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C98" s="13"/>
+      <c r="D98" s="13"/>
+      <c r="E98" s="32"/>
+      <c r="F98" s="25"/>
+      <c r="G98" s="24"/>
+    </row>
+    <row r="99" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A99" s="14"/>
+      <c r="B99" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C99" s="14"/>
+      <c r="D99" s="14"/>
+      <c r="E99" s="31"/>
+      <c r="F99" s="25"/>
+      <c r="G99" s="24"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A100" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D100" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="E100" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="F100" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="G100" s="24"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A101" s="13"/>
+      <c r="B101" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D101" s="27"/>
+      <c r="E101" s="32"/>
+      <c r="F101" s="25"/>
+      <c r="G101" s="24"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A102" s="13"/>
+      <c r="B102" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C102" s="8"/>
+      <c r="D102" s="27"/>
+      <c r="E102" s="32"/>
+      <c r="F102" s="25"/>
+      <c r="G102" s="24"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A103" s="13"/>
+      <c r="B103" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C103" s="8"/>
+      <c r="D103" s="27"/>
+      <c r="E103" s="32"/>
+      <c r="F103" s="25"/>
+      <c r="G103" s="24"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A104" s="13"/>
+      <c r="B104" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C104" s="8"/>
+      <c r="D104" s="27"/>
+      <c r="E104" s="32"/>
+      <c r="F104" s="25"/>
+      <c r="G104" s="24"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A105" s="13"/>
+      <c r="B105" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C105" s="8"/>
+      <c r="D105" s="27"/>
+      <c r="E105" s="32"/>
+      <c r="F105" s="25"/>
+      <c r="G105" s="24"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A106" s="13"/>
+      <c r="B106" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="C106" s="8"/>
+      <c r="D106" s="27"/>
+      <c r="E106" s="32"/>
+      <c r="F106" s="25"/>
+      <c r="G106" s="24"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A107" s="13"/>
+      <c r="B107" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C107" s="8"/>
+      <c r="D107" s="27"/>
+      <c r="E107" s="32"/>
+      <c r="F107" s="25"/>
+      <c r="G107" s="24"/>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A108" s="13"/>
+      <c r="B108" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C108" s="8"/>
+      <c r="D108" s="27"/>
+      <c r="E108" s="32"/>
+      <c r="F108" s="25"/>
+      <c r="G108" s="24"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A109" s="13"/>
+      <c r="B109" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C109" s="8"/>
+      <c r="D109" s="27"/>
+      <c r="E109" s="32"/>
+      <c r="F109" s="25"/>
+      <c r="G109" s="24"/>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A110" s="13"/>
+      <c r="B110" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C110" s="8"/>
+      <c r="D110" s="27"/>
+      <c r="E110" s="32"/>
+      <c r="F110" s="25"/>
+      <c r="G110" s="24"/>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A111" s="13"/>
+      <c r="B111" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C87" s="4"/>
-      <c r="D87" s="12"/>
-    </row>
-    <row r="88" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A88" s="12"/>
-      <c r="B88" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C88" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="D88" s="12"/>
-    </row>
-    <row r="89" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A89" s="12"/>
-      <c r="B89" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="C89" s="8"/>
-      <c r="D89" s="12"/>
-    </row>
-    <row r="90" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A90" s="12"/>
-      <c r="B90" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="C90" s="8"/>
-      <c r="D90" s="12"/>
-    </row>
-    <row r="91" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A91" s="13"/>
-      <c r="B91" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="C91" s="9"/>
-      <c r="D91" s="13"/>
-    </row>
-    <row r="92" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A92" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="B92" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C92" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="D92" s="14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A93" s="12"/>
-      <c r="B93" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C93" s="12"/>
-      <c r="D93" s="12"/>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A94" s="12"/>
-      <c r="B94" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C94" s="12"/>
-      <c r="D94" s="12"/>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A95" s="12"/>
-      <c r="B95" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C95" s="12"/>
-      <c r="D95" s="12"/>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A96" s="12"/>
-      <c r="B96" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C96" s="12"/>
-      <c r="D96" s="12"/>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A97" s="12"/>
-      <c r="B97" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C97" s="12"/>
-      <c r="D97" s="12"/>
-    </row>
-    <row r="98" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A98" s="12"/>
-      <c r="B98" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C98" s="12"/>
-      <c r="D98" s="12"/>
-    </row>
-    <row r="99" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A99" s="13"/>
-      <c r="B99" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="C99" s="13"/>
-      <c r="D99" s="13"/>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A100" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="B100" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C100" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="D100" s="14" t="s">
+      <c r="C111" s="8"/>
+      <c r="D111" s="27"/>
+      <c r="E111" s="32"/>
+      <c r="F111" s="25"/>
+      <c r="G111" s="24"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A112" s="13"/>
+      <c r="B112" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="C112" s="8"/>
+      <c r="D112" s="27"/>
+      <c r="E112" s="32"/>
+      <c r="F112" s="25"/>
+      <c r="G112" s="24"/>
+    </row>
+    <row r="113" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A113" s="13"/>
+      <c r="B113" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C113" s="8"/>
+      <c r="D113" s="27"/>
+      <c r="E113" s="32"/>
+      <c r="F113" s="25"/>
+      <c r="G113" s="24"/>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A114" s="13"/>
+      <c r="B114" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="C114" s="8"/>
+      <c r="D114" s="27"/>
+      <c r="E114" s="32"/>
+      <c r="F114" s="25"/>
+      <c r="G114" s="24"/>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A115" s="13"/>
+      <c r="B115" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C115" s="8"/>
+      <c r="D115" s="27"/>
+      <c r="E115" s="32"/>
+      <c r="F115" s="25"/>
+      <c r="G115" s="24"/>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A116" s="13"/>
+      <c r="B116" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C116" s="8"/>
+      <c r="D116" s="27"/>
+      <c r="E116" s="32"/>
+      <c r="F116" s="25"/>
+      <c r="G116" s="24"/>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A117" s="13"/>
+      <c r="B117" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="C117" s="8"/>
+      <c r="D117" s="27"/>
+      <c r="E117" s="32"/>
+      <c r="F117" s="25"/>
+      <c r="G117" s="24"/>
+    </row>
+    <row r="118" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A118" s="14"/>
+      <c r="B118" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C118" s="9"/>
+      <c r="D118" s="28"/>
+      <c r="E118" s="31"/>
+      <c r="F118" s="25"/>
+      <c r="G118" s="24"/>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A119" s="12" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A101" s="12"/>
-      <c r="B101" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="C101" s="4" t="s">
+      <c r="B119" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C119" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="D119" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E119" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="F119" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="G119" s="24"/>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A120" s="13"/>
+      <c r="B120" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C120" s="13"/>
+      <c r="D120" s="13"/>
+      <c r="E120" s="32"/>
+      <c r="F120" s="25"/>
+      <c r="G120" s="24"/>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A121" s="13"/>
+      <c r="B121" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C121" s="13"/>
+      <c r="D121" s="13"/>
+      <c r="E121" s="32"/>
+      <c r="F121" s="25"/>
+      <c r="G121" s="24"/>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A122" s="13"/>
+      <c r="B122" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C122" s="13"/>
+      <c r="D122" s="13"/>
+      <c r="E122" s="32"/>
+      <c r="F122" s="25"/>
+      <c r="G122" s="24"/>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A123" s="13"/>
+      <c r="B123" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C123" s="13"/>
+      <c r="D123" s="13"/>
+      <c r="E123" s="32"/>
+      <c r="F123" s="25"/>
+      <c r="G123" s="24"/>
+    </row>
+    <row r="124" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A124" s="14"/>
+      <c r="B124" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C124" s="14"/>
+      <c r="D124" s="14"/>
+      <c r="E124" s="31"/>
+      <c r="F124" s="25"/>
+      <c r="G124" s="24"/>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A125" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="B125" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C125" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="D125" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E125" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="F125" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="G125" s="24"/>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A126" s="13"/>
+      <c r="B126" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="C126" s="13"/>
+      <c r="D126" s="13"/>
+      <c r="E126" s="32"/>
+      <c r="F126" s="25"/>
+      <c r="G126" s="24"/>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A127" s="13"/>
+      <c r="B127" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="C127" s="13"/>
+      <c r="D127" s="13"/>
+      <c r="E127" s="32"/>
+      <c r="F127" s="25"/>
+      <c r="G127" s="24"/>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A128" s="13"/>
+      <c r="B128" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C128" s="13"/>
+      <c r="D128" s="13"/>
+      <c r="E128" s="32"/>
+      <c r="F128" s="25"/>
+      <c r="G128" s="24"/>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A129" s="13"/>
+      <c r="B129" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="C129" s="13"/>
+      <c r="D129" s="13"/>
+      <c r="E129" s="32"/>
+      <c r="F129" s="25"/>
+      <c r="G129" s="24"/>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A130" s="13"/>
+      <c r="B130" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C130" s="13"/>
+      <c r="D130" s="13"/>
+      <c r="E130" s="32"/>
+      <c r="F130" s="25"/>
+      <c r="G130" s="24"/>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A131" s="13"/>
+      <c r="B131" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="C131" s="13"/>
+      <c r="D131" s="13"/>
+      <c r="E131" s="32"/>
+      <c r="F131" s="25"/>
+      <c r="G131" s="24"/>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A132" s="13"/>
+      <c r="B132" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="C132" s="13"/>
+      <c r="D132" s="13"/>
+      <c r="E132" s="32"/>
+      <c r="F132" s="25"/>
+      <c r="G132" s="24"/>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A133" s="13"/>
+      <c r="B133" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C133" s="13"/>
+      <c r="D133" s="13"/>
+      <c r="E133" s="32"/>
+      <c r="F133" s="25"/>
+      <c r="G133" s="24"/>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A134" s="13"/>
+      <c r="B134" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="C134" s="13"/>
+      <c r="D134" s="13"/>
+      <c r="E134" s="32"/>
+      <c r="F134" s="25"/>
+      <c r="G134" s="24"/>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A135" s="13"/>
+      <c r="B135" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C135" s="13"/>
+      <c r="D135" s="13"/>
+      <c r="E135" s="32"/>
+      <c r="F135" s="25"/>
+      <c r="G135" s="24"/>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A136" s="13"/>
+      <c r="B136" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="C136" s="13"/>
+      <c r="D136" s="13"/>
+      <c r="E136" s="32"/>
+      <c r="F136" s="25"/>
+      <c r="G136" s="24"/>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A137" s="13"/>
+      <c r="B137" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="C137" s="13"/>
+      <c r="D137" s="13"/>
+      <c r="E137" s="32"/>
+      <c r="F137" s="25"/>
+      <c r="G137" s="24"/>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A138" s="13"/>
+      <c r="B138" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C138" s="13"/>
+      <c r="D138" s="13"/>
+      <c r="E138" s="32"/>
+      <c r="F138" s="25"/>
+      <c r="G138" s="24"/>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A139" s="13"/>
+      <c r="B139" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="C139" s="13"/>
+      <c r="D139" s="13"/>
+      <c r="E139" s="32"/>
+      <c r="F139" s="25"/>
+      <c r="G139" s="24"/>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A140" s="13"/>
+      <c r="B140" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C140" s="13"/>
+      <c r="D140" s="13"/>
+      <c r="E140" s="32"/>
+      <c r="F140" s="25"/>
+      <c r="G140" s="24"/>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A141" s="13"/>
+      <c r="B141" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="C141" s="13"/>
+      <c r="D141" s="13"/>
+      <c r="E141" s="32"/>
+      <c r="F141" s="25"/>
+      <c r="G141" s="24"/>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A142" s="13"/>
+      <c r="B142" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="C142" s="13"/>
+      <c r="D142" s="13"/>
+      <c r="E142" s="32"/>
+      <c r="F142" s="25"/>
+      <c r="G142" s="24"/>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A143" s="13"/>
+      <c r="B143" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C143" s="13"/>
+      <c r="D143" s="13"/>
+      <c r="E143" s="32"/>
+      <c r="F143" s="25"/>
+      <c r="G143" s="24"/>
+    </row>
+    <row r="144" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A144" s="14"/>
+      <c r="B144" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="C144" s="14"/>
+      <c r="D144" s="14"/>
+      <c r="E144" s="31"/>
+      <c r="F144" s="25"/>
+      <c r="G144" s="24"/>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A145" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="B145" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C145" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D145" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="D101" s="12"/>
-    </row>
-    <row r="102" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A102" s="12"/>
-      <c r="B102" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="C102" s="8"/>
-      <c r="D102" s="12"/>
-    </row>
-    <row r="103" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A103" s="12"/>
-      <c r="B103" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="C103" s="8"/>
-      <c r="D103" s="12"/>
-    </row>
-    <row r="104" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A104" s="12"/>
-      <c r="B104" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="C104" s="8"/>
-      <c r="D104" s="12"/>
-    </row>
-    <row r="105" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A105" s="12"/>
-      <c r="B105" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="C105" s="8"/>
-      <c r="D105" s="12"/>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A106" s="12"/>
-      <c r="B106" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="C106" s="8"/>
-      <c r="D106" s="12"/>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A107" s="12"/>
-      <c r="B107" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="C107" s="8"/>
-      <c r="D107" s="12"/>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A108" s="12"/>
-      <c r="B108" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="C108" s="8"/>
-      <c r="D108" s="12"/>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A109" s="12"/>
-      <c r="B109" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="C109" s="8"/>
-      <c r="D109" s="12"/>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A110" s="12"/>
-      <c r="B110" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="C110" s="8"/>
-      <c r="D110" s="12"/>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A111" s="12"/>
-      <c r="B111" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C111" s="8"/>
-      <c r="D111" s="12"/>
-    </row>
-    <row r="112" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A112" s="12"/>
-      <c r="B112" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="C112" s="8"/>
-      <c r="D112" s="12"/>
-    </row>
-    <row r="113" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="A113" s="12"/>
-      <c r="B113" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="C113" s="8"/>
-      <c r="D113" s="12"/>
-    </row>
-    <row r="114" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A114" s="12"/>
-      <c r="B114" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="C114" s="8"/>
-      <c r="D114" s="12"/>
-    </row>
-    <row r="115" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A115" s="12"/>
-      <c r="B115" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="C115" s="8"/>
-      <c r="D115" s="12"/>
-    </row>
-    <row r="116" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A116" s="12"/>
-      <c r="B116" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="C116" s="8"/>
-      <c r="D116" s="12"/>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A117" s="12"/>
-      <c r="B117" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="C117" s="8"/>
-      <c r="D117" s="12"/>
-    </row>
-    <row r="118" spans="1:4" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A118" s="13"/>
-      <c r="B118" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="C118" s="9"/>
-      <c r="D118" s="13"/>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A119" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="B119" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="C119" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="D119" s="14"/>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A120" s="12"/>
-      <c r="B120" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="C120" s="12"/>
-      <c r="D120" s="12"/>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A121" s="12"/>
-      <c r="B121" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="C121" s="12"/>
-      <c r="D121" s="12"/>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A122" s="12"/>
-      <c r="B122" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="C122" s="12"/>
-      <c r="D122" s="12"/>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A123" s="12"/>
-      <c r="B123" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="C123" s="12"/>
-      <c r="D123" s="12"/>
-    </row>
-    <row r="124" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A124" s="13"/>
-      <c r="B124" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="C124" s="13"/>
-      <c r="D124" s="13"/>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A125" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="B125" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="C125" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="D125" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A126" s="12"/>
-      <c r="B126" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="C126" s="12"/>
-      <c r="D126" s="12"/>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A127" s="12"/>
-      <c r="B127" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="C127" s="12"/>
-      <c r="D127" s="12"/>
-    </row>
-    <row r="128" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A128" s="12"/>
-      <c r="B128" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="C128" s="12"/>
-      <c r="D128" s="12"/>
-    </row>
-    <row r="129" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A129" s="12"/>
-      <c r="B129" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="C129" s="12"/>
-      <c r="D129" s="12"/>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A130" s="12"/>
-      <c r="B130" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="C130" s="12"/>
-      <c r="D130" s="12"/>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A131" s="12"/>
-      <c r="B131" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="C131" s="12"/>
-      <c r="D131" s="12"/>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A132" s="12"/>
-      <c r="B132" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="C132" s="12"/>
-      <c r="D132" s="12"/>
-    </row>
-    <row r="133" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A133" s="12"/>
-      <c r="B133" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="C133" s="12"/>
-      <c r="D133" s="12"/>
-    </row>
-    <row r="134" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A134" s="12"/>
-      <c r="B134" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="C134" s="12"/>
-      <c r="D134" s="12"/>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A135" s="12"/>
-      <c r="B135" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C135" s="12"/>
-      <c r="D135" s="12"/>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A136" s="12"/>
-      <c r="B136" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="C136" s="12"/>
-      <c r="D136" s="12"/>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A137" s="12"/>
-      <c r="B137" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="C137" s="12"/>
-      <c r="D137" s="12"/>
-    </row>
-    <row r="138" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A138" s="12"/>
-      <c r="B138" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="C138" s="12"/>
-      <c r="D138" s="12"/>
-    </row>
-    <row r="139" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A139" s="12"/>
-      <c r="B139" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="C139" s="12"/>
-      <c r="D139" s="12"/>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A140" s="12"/>
-      <c r="B140" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="C140" s="12"/>
-      <c r="D140" s="12"/>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A141" s="12"/>
-      <c r="B141" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="C141" s="12"/>
-      <c r="D141" s="12"/>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A142" s="12"/>
-      <c r="B142" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="C142" s="12"/>
-      <c r="D142" s="12"/>
-    </row>
-    <row r="143" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A143" s="12"/>
-      <c r="B143" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="C143" s="12"/>
-      <c r="D143" s="12"/>
-    </row>
-    <row r="144" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A144" s="13"/>
-      <c r="B144" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="C144" s="13"/>
-      <c r="D144" s="13"/>
-    </row>
-    <row r="145" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A145" s="14" t="s">
+      <c r="E145" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="F145" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="G145" s="24"/>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A146" s="13"/>
+      <c r="B146" s="10" t="s">
         <v>175</v>
-      </c>
-      <c r="B145" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C145" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="D145" s="14" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A146" s="12"/>
-      <c r="B146" s="10" t="s">
-        <v>176</v>
       </c>
       <c r="C146" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D146" s="12"/>
-    </row>
-    <row r="147" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A147" s="12"/>
+      <c r="D146" s="13"/>
+      <c r="E146" s="32"/>
+      <c r="F146" s="25"/>
+      <c r="G146" s="24"/>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A147" s="13"/>
       <c r="B147" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C147" s="8"/>
+      <c r="D147" s="13"/>
+      <c r="E147" s="32"/>
+      <c r="F147" s="25"/>
+      <c r="G147" s="24"/>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A148" s="13"/>
+      <c r="B148" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C148" s="8"/>
+      <c r="D148" s="13"/>
+      <c r="E148" s="32"/>
+      <c r="F148" s="25"/>
+      <c r="G148" s="24"/>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A149" s="13"/>
+      <c r="B149" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="C147" s="8"/>
-      <c r="D147" s="12"/>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A148" s="12"/>
-      <c r="B148" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C148" s="8"/>
-      <c r="D148" s="12"/>
-    </row>
-    <row r="149" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A149" s="12"/>
-      <c r="B149" s="10" t="s">
+      <c r="C149" s="8"/>
+      <c r="D149" s="13"/>
+      <c r="E149" s="32"/>
+      <c r="F149" s="25"/>
+      <c r="G149" s="24"/>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A150" s="13"/>
+      <c r="B150" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="C149" s="8"/>
-      <c r="D149" s="12"/>
-    </row>
-    <row r="150" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A150" s="12"/>
-      <c r="B150" s="10" t="s">
+      <c r="C150" s="8"/>
+      <c r="D150" s="13"/>
+      <c r="E150" s="32"/>
+      <c r="F150" s="25"/>
+      <c r="G150" s="24"/>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A151" s="13"/>
+      <c r="B151" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C151" s="8"/>
+      <c r="D151" s="13"/>
+      <c r="E151" s="32"/>
+      <c r="F151" s="25"/>
+      <c r="G151" s="24"/>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A152" s="13"/>
+      <c r="B152" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C150" s="8"/>
-      <c r="D150" s="12"/>
-    </row>
-    <row r="151" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A151" s="12"/>
-      <c r="B151" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="C151" s="8"/>
-      <c r="D151" s="12"/>
-    </row>
-    <row r="152" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A152" s="12"/>
-      <c r="B152" s="10" t="s">
+      <c r="C152" s="8"/>
+      <c r="D152" s="13"/>
+      <c r="E152" s="32"/>
+      <c r="F152" s="25"/>
+      <c r="G152" s="24"/>
+    </row>
+    <row r="153" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A153" s="14"/>
+      <c r="B153" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="C152" s="8"/>
-      <c r="D152" s="12"/>
-    </row>
-    <row r="153" spans="1:4" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A153" s="13"/>
-      <c r="B153" s="11" t="s">
-        <v>181</v>
-      </c>
       <c r="C153" s="9"/>
-      <c r="D153" s="13"/>
+      <c r="D153" s="14"/>
+      <c r="E153" s="31"/>
+      <c r="F153" s="25"/>
+      <c r="G153" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
+  <mergeCells count="74">
+    <mergeCell ref="E119:E124"/>
+    <mergeCell ref="E125:E144"/>
+    <mergeCell ref="E145:E153"/>
+    <mergeCell ref="F119:G124"/>
+    <mergeCell ref="F125:G144"/>
+    <mergeCell ref="F145:G153"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="E6:E13"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="E22:E26"/>
+    <mergeCell ref="E27:E34"/>
+    <mergeCell ref="E35:E49"/>
+    <mergeCell ref="E50:E70"/>
+    <mergeCell ref="E71:E77"/>
+    <mergeCell ref="E78:E85"/>
+    <mergeCell ref="E86:E91"/>
+    <mergeCell ref="E92:E99"/>
+    <mergeCell ref="E100:E118"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F4:G5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="F100:G118"/>
+    <mergeCell ref="F6:G13"/>
+    <mergeCell ref="F14:G17"/>
+    <mergeCell ref="F18:G21"/>
+    <mergeCell ref="F22:G26"/>
+    <mergeCell ref="F27:G34"/>
+    <mergeCell ref="F35:G49"/>
+    <mergeCell ref="F50:G70"/>
+    <mergeCell ref="F71:G77"/>
+    <mergeCell ref="F78:G85"/>
+    <mergeCell ref="F86:G91"/>
+    <mergeCell ref="F92:G99"/>
+    <mergeCell ref="C6:C13"/>
+    <mergeCell ref="D6:D13"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="F2:G3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="C71:C77"/>
+    <mergeCell ref="D71:D77"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="C22:C26"/>
+    <mergeCell ref="D22:D26"/>
+    <mergeCell ref="C27:C34"/>
+    <mergeCell ref="D27:D34"/>
+    <mergeCell ref="C35:C49"/>
+    <mergeCell ref="D35:D49"/>
+    <mergeCell ref="A50:A70"/>
+    <mergeCell ref="C78:C85"/>
+    <mergeCell ref="D78:D85"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="D86:D91"/>
+    <mergeCell ref="A92:A99"/>
+    <mergeCell ref="C92:C99"/>
+    <mergeCell ref="D92:D99"/>
     <mergeCell ref="A145:A153"/>
     <mergeCell ref="D145:D153"/>
     <mergeCell ref="A100:A118"/>
@@ -3293,33 +4093,6 @@
     <mergeCell ref="A125:A144"/>
     <mergeCell ref="C125:C144"/>
     <mergeCell ref="D125:D144"/>
-    <mergeCell ref="C78:C85"/>
-    <mergeCell ref="D78:D85"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="D86:D91"/>
-    <mergeCell ref="A92:A99"/>
-    <mergeCell ref="C92:C99"/>
-    <mergeCell ref="D92:D99"/>
-    <mergeCell ref="C27:C34"/>
-    <mergeCell ref="D27:D34"/>
-    <mergeCell ref="C35:C49"/>
-    <mergeCell ref="D35:D49"/>
-    <mergeCell ref="A50:A70"/>
-    <mergeCell ref="C71:C77"/>
-    <mergeCell ref="D71:D77"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="C22:C26"/>
-    <mergeCell ref="D22:D26"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="C6:C13"/>
-    <mergeCell ref="D6:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>